<commit_message>
Wrote function to strip out k__ notation
</commit_message>
<xml_diff>
--- a/test/fixtures/Test_NCBItaxa_good.xlsx
+++ b/test/fixtures/Test_NCBItaxa_good.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc2017/Documents/MyRepos/safedata_validator/test/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD1C835-55FD-CD48-A68C-7A1DAF3D0A1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D4ABE6-2F4D-3F43-9402-ED1655069542}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27880" windowHeight="15840" xr2:uid="{819B57D8-7F20-471A-9405-EB60A28E68AA}"/>
   </bookViews>
@@ -523,7 +523,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Hopefully this removes old file
</commit_message>
<xml_diff>
--- a/test/fixtures/Test_NCBItaxa_good.xlsx
+++ b/test/fixtures/Test_NCBItaxa_good.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc2017/Documents/MyRepos/safedata_validator/test/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D4ABE6-2F4D-3F43-9402-ED1655069542}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC140339-AC62-2E4D-893C-75726DA0FF66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27880" windowHeight="15840" xr2:uid="{819B57D8-7F20-471A-9405-EB60A28E68AA}"/>
   </bookViews>
@@ -523,7 +523,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -537,6 +537,7 @@
     <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Completed script to make truncated database for testing
</commit_message>
<xml_diff>
--- a/test/fixtures/Test_NCBItaxa_good.xlsx
+++ b/test/fixtures/Test_NCBItaxa_good.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc2017/Documents/MyRepos/safedata_validator/test/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC140339-AC62-2E4D-893C-75726DA0FF66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8B8880-9527-0E48-8E41-6F097C76A44A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27880" windowHeight="15840" xr2:uid="{819B57D8-7F20-471A-9405-EB60A28E68AA}"/>
+    <workbookView xWindow="-20" yWindow="2560" windowWidth="27880" windowHeight="15840" xr2:uid="{819B57D8-7F20-471A-9405-EB60A28E68AA}"/>
   </bookViews>
   <sheets>
     <sheet name="NCBITaxa" sheetId="1" r:id="rId1"/>
@@ -523,7 +523,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added a check on the comments field
</commit_message>
<xml_diff>
--- a/test/fixtures/Test_NCBItaxa_good.xlsx
+++ b/test/fixtures/Test_NCBItaxa_good.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc2017/Documents/MyRepos/safedata_validator/test/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8B8880-9527-0E48-8E41-6F097C76A44A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58527A07-AE74-9E4A-AC99-B840E2666B24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="2560" windowWidth="27880" windowHeight="15840" xr2:uid="{819B57D8-7F20-471A-9405-EB60A28E68AA}"/>
+    <workbookView xWindow="0" yWindow="2160" windowWidth="27880" windowHeight="15840" xr2:uid="{819B57D8-7F20-471A-9405-EB60A28E68AA}"/>
   </bookViews>
   <sheets>
     <sheet name="NCBITaxa" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
   <si>
     <t>Kingdom</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>Rhodoplanes 2</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>This has never been cultured so has an unusual name</t>
   </si>
 </sst>
 </file>
@@ -204,8 +210,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6973E772-319E-4D19-B398-4AADD9788389}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -537,10 +546,10 @@
     <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -568,8 +577,11 @@
       <c r="I1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -595,7 +607,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -621,7 +633,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -647,7 +659,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -673,7 +685,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -699,7 +711,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -725,7 +737,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -751,7 +763,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -777,7 +789,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -803,7 +815,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -827,6 +839,9 @@
       </c>
       <c r="I11" t="s">
         <v>13</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>